<commit_message>
Bug fix, Design and Exit button
</commit_message>
<xml_diff>
--- a/login_file.xlsx
+++ b/login_file.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niron\Desktop\BirdsControl\BirdsControl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gofma\OneDrive\שולחן העבודה\BirdsControl\BirdsControl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD45D997-2E1A-4AB4-9088-1C37D5D8DA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A81C1D-3F17-4045-A84F-5F6B42189218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{056BD8C1-C541-4C84-A611-2C9B857187B6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{056BD8C1-C541-4C84-A611-2C9B857187B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -415,19 +415,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04331750-A4CC-4FB1-9F16-817AAA4C0DCC}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.3984375" customWidth="1"/>
-    <col min="3" max="3" width="20.3984375" customWidth="1"/>
+    <col min="2" max="2" width="15.4140625" customWidth="1"/>
+    <col min="3" max="3" width="20.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,7 +438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -449,7 +449,7 @@
         <v>209375906</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -460,7 +460,7 @@
         <v>209375908</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -471,7 +471,7 @@
         <v>209375909</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -482,7 +482,7 @@
         <v>208212191</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -493,7 +493,7 @@
         <v>208212192</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -504,7 +504,7 @@
         <v>209375904</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -515,7 +515,7 @@
         <v>315434621</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -524,6 +524,17 @@
       </c>
       <c r="C9">
         <v>209375806</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>